<commit_message>
warning: in the working copy of 'htc_ xgboost.ipynb', LF will be replaced by CRLF the next time Git touches it
</commit_message>
<xml_diff>
--- a/HLA_Attribute_Classification.xlsx
+++ b/HLA_Attribute_Classification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lince\OneDrive\Desktop\htc-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6F3383-A522-40E4-A58A-E1D3A4AF6144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA1DBF2-1DDB-4B71-8DC0-E9890FD1A7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -745,13 +745,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.33203125" customWidth="1"/>
   </cols>
@@ -955,7 +955,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B19" t="s">
@@ -966,7 +966,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B20" t="s">

</xml_diff>

<commit_message>
all attributed added to excel
</commit_message>
<xml_diff>
--- a/HLA_Attribute_Classification.xlsx
+++ b/HLA_Attribute_Classification.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lince\OneDrive\Desktop\htc-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA1DBF2-1DDB-4B71-8DC0-E9890FD1A7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B739D1-9406-4BF9-8649-EB573EC07D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="120">
   <si>
     <t>Attribute</t>
   </si>
@@ -374,6 +387,12 @@
   </si>
   <si>
     <t>Duplicate of another HLA variable</t>
+  </si>
+  <si>
+    <t>tce_imm_match</t>
+  </si>
+  <si>
+    <t>cyto_score_detail</t>
   </si>
 </sst>
 </file>
@@ -394,18 +413,12 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -435,12 +448,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -743,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -768,7 +780,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -779,7 +791,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
@@ -790,7 +802,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
@@ -812,7 +824,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
@@ -823,7 +835,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
@@ -834,7 +846,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8" t="s">
@@ -845,7 +857,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
@@ -856,7 +868,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
@@ -867,7 +879,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">
@@ -889,7 +901,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>25</v>
       </c>
       <c r="B13" t="s">
@@ -900,7 +912,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
       <c r="B14" t="s">
@@ -911,7 +923,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>30</v>
       </c>
       <c r="B15" t="s">
@@ -922,7 +934,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>32</v>
       </c>
       <c r="B16" t="s">
@@ -933,7 +945,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>33</v>
       </c>
       <c r="B17" t="s">
@@ -944,7 +956,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>35</v>
       </c>
       <c r="B18" t="s">
@@ -955,7 +967,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>37</v>
       </c>
       <c r="B19" t="s">
@@ -966,7 +978,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>39</v>
       </c>
       <c r="B20" t="s">
@@ -1425,6 +1437,16 @@
       </c>
       <c r="C61" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>